<commit_message>
New Work organization v3
</commit_message>
<xml_diff>
--- a/data/xlsx/speech.xlsx
+++ b/data/xlsx/speech.xlsx
@@ -4208,12 +4208,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Colombia_2014_Juan_Manuel_Santos.pdf</t>
+          <t>Colombia_2014_JuanManuel_Santos.pdf</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Colombia_2014_Juan_Manuel_Santos.txt</t>
+          <t>Colombia_2014_JuanManuel_Santos.txt</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Juan_Manuel_Santos</t>
+          <t>JuanManuel_Santos</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4475,12 +4475,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Colombia_2018_Juan_Manuel_Santos.pdf</t>
+          <t>Colombia_2018_JuanManuel_Santos.pdf</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Colombia_2018_Juan_Manuel_Santos.txt</t>
+          <t>Colombia_2018_JuanManuel_Santos.txt</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4490,7 +4490,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Juan_Manuel_Santos</t>
+          <t>JuanManuel_Santos</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">

</xml_diff>